<commit_message>
markdown formatting; separate internal and external rendering options
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -7891,6 +7891,14 @@
         <v>664</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>619</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -7989,6 +7997,14 @@
         <v>674</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>619</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
major reorg to study 2, moving all preprocessing to 1_preprocess.qmd
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="677">
   <si>
     <t xml:space="preserve">Tab</t>
   </si>
@@ -1881,6 +1881,9 @@
   </si>
   <si>
     <t xml:space="preserve">The length of the gaming session in minutes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sessionEnd</t>
   </si>
   <si>
     <t xml:space="preserve">genre</t>
@@ -2515,7 +2518,7 @@
     </row>
     <row r="11" ht="50" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -7435,20 +7438,31 @@
         <v>616</v>
       </c>
       <c r="B9" t="s">
-        <v>617</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>618</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>617</v>
+      </c>
+      <c r="B10" t="s">
+        <v>618</v>
+      </c>
+      <c r="C10" t="s">
         <v>619</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
         <v>620</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>621</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7564,20 +7578,31 @@
         <v>616</v>
       </c>
       <c r="B9" t="s">
-        <v>621</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>618</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B10" t="s">
         <v>622</v>
       </c>
       <c r="C10" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>620</v>
+      </c>
+      <c r="B11" t="s">
+        <v>623</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7595,7 +7620,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="8.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="12.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="90.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="250.71" hidden="0" customWidth="1"/>
   </cols>
@@ -7646,10 +7671,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B5" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -7657,10 +7682,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -7668,21 +7693,21 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B7" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C7" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B8" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
@@ -7690,10 +7715,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B9" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
@@ -7701,7 +7726,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B10" t="s">
         <v>611</v>
@@ -7712,12 +7737,34 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B11" t="s">
-        <v>632</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>616</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>620</v>
+      </c>
+      <c r="B13" t="s">
+        <v>633</v>
+      </c>
+      <c r="C13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7757,10 +7804,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B3" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4">
@@ -7768,87 +7815,87 @@
         <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B5" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B6" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B7" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B9" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B10" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B11" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B12" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B13" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B14" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="15">
@@ -7856,44 +7903,44 @@
         <v>563</v>
       </c>
       <c r="B15" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B16" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B17" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B18" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B19" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
@@ -7943,10 +7990,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B4" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="5">
@@ -7954,7 +8001,7 @@
         <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6">
@@ -7962,15 +8009,15 @@
         <v>608</v>
       </c>
       <c r="B6" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B7" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="8">
@@ -7978,7 +8025,7 @@
         <v>612</v>
       </c>
       <c r="B8" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="9">
@@ -7986,22 +8033,30 @@
         <v>614</v>
       </c>
       <c r="B9" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>673</v>
+        <v>616</v>
       </c>
       <c r="B10" t="s">
-        <v>674</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>619</v>
+        <v>674</v>
       </c>
       <c r="B11" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>620</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>